<commit_message>
add zephyr-rts.py for testing
</commit_message>
<xml_diff>
--- a/io/generator_fuel_assumptions.xlsx
+++ b/io/generator_fuel_assumptions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickbrown/github/zephyr/io/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pbrown/github/zephyr/io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7FC6E9-8511-B740-9AE2-904D97BB9494}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204F307F-C4BB-4A46-8848-F0C2B54C2F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-5400" windowWidth="25600" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Generators_rawUSD" sheetId="9" r:id="rId1"/>
@@ -38,13 +38,24 @@
     <definedName name="inflator_2018">Financials!$E$12</definedName>
     <definedName name="wacc">Financials!$A$4</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -173,7 +184,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="286">
   <si>
     <t>Technology</t>
   </si>
@@ -1022,13 +1033,22 @@
   </si>
   <si>
     <t>PHS_0</t>
+  </si>
+  <si>
+    <t>Coal</t>
+  </si>
+  <si>
+    <t>coal</t>
+  </si>
+  <si>
+    <t>Source_heatrate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1086,11 +1106,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1407,15 +1426,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P59"/>
+  <dimension ref="A1:P60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A8" sqref="A8"/>
-      <selection pane="topRight" activeCell="A59" sqref="A58:XFD59"/>
+      <selection pane="topRight" activeCell="H62" sqref="H62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
@@ -1433,7 +1452,7 @@
     <col min="14" max="14" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1483,7 +1502,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1527,7 +1546,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>42</v>
       </c>
@@ -1568,7 +1587,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1620,7 +1639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -1634,7 +1653,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:E59" si="0">((D5*(1+D5)^C5)/((1+D5)^C5-1))</f>
+        <f t="shared" ref="E5:E60" si="0">((D5*(1+D5)^C5)/((1+D5)^C5-1))</f>
         <v>6.7439028038694573E-2</v>
       </c>
       <c r="F5">
@@ -1672,7 +1691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>105</v>
       </c>
@@ -1724,7 +1743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>110</v>
       </c>
@@ -1776,7 +1795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>127</v>
       </c>
@@ -1828,7 +1847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>128</v>
       </c>
@@ -1880,7 +1899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>129</v>
       </c>
@@ -1932,7 +1951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>130</v>
       </c>
@@ -1984,7 +2003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -2036,7 +2055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>111</v>
       </c>
@@ -2088,7 +2107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>112</v>
       </c>
@@ -2140,7 +2159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>113</v>
       </c>
@@ -2192,7 +2211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>131</v>
       </c>
@@ -2244,7 +2263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>132</v>
       </c>
@@ -2296,7 +2315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>133</v>
       </c>
@@ -2348,7 +2367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>134</v>
       </c>
@@ -2400,7 +2419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -2452,7 +2471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>122</v>
       </c>
@@ -2504,7 +2523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>123</v>
       </c>
@@ -2556,7 +2575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>124</v>
       </c>
@@ -2608,7 +2627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>125</v>
       </c>
@@ -2660,7 +2679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>216</v>
       </c>
@@ -2712,7 +2731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>255</v>
       </c>
@@ -2755,7 +2774,7 @@
       <c r="M26" t="s">
         <v>25</v>
       </c>
-      <c r="N26" s="4" t="s">
+      <c r="N26" s="3" t="s">
         <v>261</v>
       </c>
       <c r="O26">
@@ -2765,7 +2784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>143</v>
       </c>
@@ -2816,7 +2835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -2870,7 +2889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>2</v>
       </c>
@@ -2924,7 +2943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>101</v>
       </c>
@@ -2978,7 +2997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>196</v>
       </c>
@@ -3032,7 +3051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>197</v>
       </c>
@@ -3086,7 +3105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>102</v>
       </c>
@@ -3140,7 +3159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>103</v>
       </c>
@@ -3194,7 +3213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>114</v>
       </c>
@@ -3248,7 +3267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>115</v>
       </c>
@@ -3302,7 +3321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>116</v>
       </c>
@@ -3356,7 +3375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:16">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>117</v>
       </c>
@@ -3410,7 +3429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:16">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -3462,7 +3481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>106</v>
       </c>
@@ -3514,7 +3533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>198</v>
       </c>
@@ -3566,7 +3585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:16">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>199</v>
       </c>
@@ -3618,7 +3637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>107</v>
       </c>
@@ -3670,7 +3689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:16">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>109</v>
       </c>
@@ -3722,7 +3741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:16">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>118</v>
       </c>
@@ -3774,7 +3793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:16">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>119</v>
       </c>
@@ -3826,7 +3845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:16">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>120</v>
       </c>
@@ -3878,7 +3897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:16">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>121</v>
       </c>
@@ -3930,7 +3949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:16">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>136</v>
       </c>
@@ -3982,7 +4001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:16">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>135</v>
       </c>
@@ -4034,7 +4053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:16">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>137</v>
       </c>
@@ -4086,7 +4105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:16">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>138</v>
       </c>
@@ -4138,7 +4157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:16">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>139</v>
       </c>
@@ -4190,7 +4209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:16">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>140</v>
       </c>
@@ -4242,7 +4261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:16">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>141</v>
       </c>
@@ -4294,7 +4313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:16">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>142</v>
       </c>
@@ -4346,7 +4365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:16">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>201</v>
       </c>
@@ -4398,7 +4417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:16">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>263</v>
       </c>
@@ -4450,7 +4469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:16">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>264</v>
       </c>
@@ -4468,7 +4487,7 @@
         <v>6.7439028038694573E-2</v>
       </c>
       <c r="F59">
-        <f t="shared" ref="F59" si="13">B59*E59</f>
+        <f t="shared" ref="F59:F60" si="13">B59*E59</f>
         <v>337.19514019347287</v>
       </c>
       <c r="G59">
@@ -4499,6 +4518,58 @@
         <v>2017</v>
       </c>
       <c r="P59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>283</v>
+      </c>
+      <c r="B60">
+        <v>10000</v>
+      </c>
+      <c r="C60">
+        <v>25</v>
+      </c>
+      <c r="D60">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="0"/>
+        <v>6.7439028038694573E-2</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="13"/>
+        <v>674.39028038694573</v>
+      </c>
+      <c r="G60">
+        <v>11</v>
+      </c>
+      <c r="H60">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="I60">
+        <v>12</v>
+      </c>
+      <c r="J60">
+        <v>0.25</v>
+      </c>
+      <c r="K60">
+        <v>0.25</v>
+      </c>
+      <c r="L60">
+        <v>0</v>
+      </c>
+      <c r="M60" t="s">
+        <v>284</v>
+      </c>
+      <c r="N60" t="s">
+        <v>262</v>
+      </c>
+      <c r="O60">
+        <v>2017</v>
+      </c>
+      <c r="P60">
         <v>1</v>
       </c>
     </row>
@@ -4514,13 +4585,13 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
@@ -4528,7 +4599,7 @@
     <col min="5" max="5" width="55.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -4542,13 +4613,13 @@
         <v>37</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>285</v>
       </c>
       <c r="F1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -4559,7 +4630,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>30</v>
       </c>
@@ -4567,7 +4638,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -4587,7 +4658,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -4604,7 +4675,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -4615,7 +4686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>233</v>
       </c>
@@ -4635,7 +4706,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>234</v>
       </c>
@@ -4655,7 +4726,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>230</v>
       </c>
@@ -4675,7 +4746,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>231</v>
       </c>
@@ -4695,7 +4766,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>232</v>
       </c>
@@ -4715,7 +4786,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>221</v>
       </c>
@@ -4735,7 +4806,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>222</v>
       </c>
@@ -4755,7 +4826,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>223</v>
       </c>
@@ -4775,7 +4846,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>218</v>
       </c>
@@ -4795,7 +4866,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>219</v>
       </c>
@@ -4815,7 +4886,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>220</v>
       </c>
@@ -4835,7 +4906,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>224</v>
       </c>
@@ -4855,7 +4926,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>225</v>
       </c>
@@ -4875,7 +4946,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>226</v>
       </c>
@@ -4895,7 +4966,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>227</v>
       </c>
@@ -4915,7 +4986,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>228</v>
       </c>
@@ -4935,7 +5006,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>229</v>
       </c>
@@ -4955,7 +5026,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>273</v>
       </c>
@@ -4972,7 +5043,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>274</v>
       </c>
@@ -4989,7 +5060,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>275</v>
       </c>
@@ -5006,7 +5077,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>276</v>
       </c>
@@ -5023,7 +5094,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>277</v>
       </c>
@@ -5040,7 +5111,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>278</v>
       </c>
@@ -5057,7 +5128,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>279</v>
       </c>
@@ -5074,7 +5145,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>280</v>
       </c>
@@ -5091,7 +5162,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>281</v>
       </c>
@@ -5105,6 +5176,26 @@
         <v>36</v>
       </c>
       <c r="F32">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>284</v>
+      </c>
+      <c r="B33">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C33">
+        <v>100</v>
+      </c>
+      <c r="D33" t="s">
+        <v>262</v>
+      </c>
+      <c r="E33" t="s">
+        <v>262</v>
+      </c>
+      <c r="F33">
         <v>2017</v>
       </c>
     </row>
@@ -5115,13 +5206,13 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
@@ -5129,7 +5220,7 @@
     <col min="5" max="5" width="55.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -5149,7 +5240,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -5160,7 +5251,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>30</v>
       </c>
@@ -5168,7 +5259,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f>Fuels_rawUSD!A4</f>
         <v>naturalgas</v>
@@ -5193,7 +5284,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f>Fuels_rawUSD!A5</f>
         <v>uranium</v>
@@ -5218,7 +5309,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f>Fuels_rawUSD!A6</f>
         <v>none</v>
@@ -5243,7 +5334,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f>Fuels_rawUSD!A7</f>
         <v>naturalgas_2017</v>
@@ -5268,7 +5359,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f>Fuels_rawUSD!A8</f>
         <v>naturalgas_2018</v>
@@ -5293,7 +5384,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
         <f>Fuels_rawUSD!A9</f>
         <v>naturalgas_2020_low</v>
@@ -5318,7 +5409,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f>Fuels_rawUSD!A10</f>
         <v>naturalgas_2020_mid</v>
@@ -5343,7 +5434,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
         <f>Fuels_rawUSD!A11</f>
         <v>naturalgas_2020_high</v>
@@ -5368,7 +5459,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
         <f>Fuels_rawUSD!A12</f>
         <v>naturalgas_2025_low</v>
@@ -5393,7 +5484,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
         <f>Fuels_rawUSD!A13</f>
         <v>naturalgas_2025_mid</v>
@@ -5418,7 +5509,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="str">
         <f>Fuels_rawUSD!A14</f>
         <v>naturalgas_2025_high</v>
@@ -5443,7 +5534,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
         <f>Fuels_rawUSD!A15</f>
         <v>naturalgas_2030_low</v>
@@ -5468,7 +5559,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
         <f>Fuels_rawUSD!A16</f>
         <v>naturalgas_2030_mid</v>
@@ -5493,7 +5584,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="str">
         <f>Fuels_rawUSD!A17</f>
         <v>naturalgas_2030_high</v>
@@ -5518,7 +5609,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
         <f>Fuels_rawUSD!A18</f>
         <v>naturalgas_2040_low</v>
@@ -5543,7 +5634,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="str">
         <f>Fuels_rawUSD!A19</f>
         <v>naturalgas_2040_mid</v>
@@ -5568,7 +5659,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="str">
         <f>Fuels_rawUSD!A20</f>
         <v>naturalgas_2040_high</v>
@@ -5593,7 +5684,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="str">
         <f>Fuels_rawUSD!A21</f>
         <v>naturalgas_2050_low</v>
@@ -5618,7 +5709,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="str">
         <f>Fuels_rawUSD!A22</f>
         <v>naturalgas_2050_mid</v>
@@ -5643,7 +5734,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
         <f>Fuels_rawUSD!A23</f>
         <v>naturalgas_2050_high</v>
@@ -5665,6 +5756,256 @@
         <v>https://www.eia.gov/environment/emissions/co2_vol_mass.php</v>
       </c>
       <c r="F23">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="str">
+        <f>Fuels_rawUSD!A24</f>
+        <v>naturalgas_2MMbtu</v>
+      </c>
+      <c r="B24">
+        <f>Fuels_rawUSD!B24*inflator_2017</f>
+        <v>2E-3</v>
+      </c>
+      <c r="C24">
+        <f>Fuels_rawUSD!C24</f>
+        <v>53.07</v>
+      </c>
+      <c r="D24">
+        <f>Fuels_rawUSD!D24</f>
+        <v>0</v>
+      </c>
+      <c r="E24" t="str">
+        <f>Fuels_rawUSD!E24</f>
+        <v>https://www.eia.gov/environment/emissions/co2_vol_mass.php</v>
+      </c>
+      <c r="F24">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="str">
+        <f>Fuels_rawUSD!A25</f>
+        <v>naturalgas_3MMbtu</v>
+      </c>
+      <c r="B25">
+        <f>Fuels_rawUSD!B25*inflator_2017</f>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C25">
+        <f>Fuels_rawUSD!C25</f>
+        <v>53.07</v>
+      </c>
+      <c r="D25">
+        <f>Fuels_rawUSD!D25</f>
+        <v>0</v>
+      </c>
+      <c r="E25" t="str">
+        <f>Fuels_rawUSD!E25</f>
+        <v>https://www.eia.gov/environment/emissions/co2_vol_mass.php</v>
+      </c>
+      <c r="F25">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="str">
+        <f>Fuels_rawUSD!A26</f>
+        <v>naturalgas_4MMbtu</v>
+      </c>
+      <c r="B26">
+        <f>Fuels_rawUSD!B26*inflator_2017</f>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C26">
+        <f>Fuels_rawUSD!C26</f>
+        <v>53.07</v>
+      </c>
+      <c r="D26">
+        <f>Fuels_rawUSD!D26</f>
+        <v>0</v>
+      </c>
+      <c r="E26" t="str">
+        <f>Fuels_rawUSD!E26</f>
+        <v>https://www.eia.gov/environment/emissions/co2_vol_mass.php</v>
+      </c>
+      <c r="F26">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="str">
+        <f>Fuels_rawUSD!A27</f>
+        <v>naturalgas_5MMbtu</v>
+      </c>
+      <c r="B27">
+        <f>Fuels_rawUSD!B27*inflator_2017</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C27">
+        <f>Fuels_rawUSD!C27</f>
+        <v>53.07</v>
+      </c>
+      <c r="D27">
+        <f>Fuels_rawUSD!D27</f>
+        <v>0</v>
+      </c>
+      <c r="E27" t="str">
+        <f>Fuels_rawUSD!E27</f>
+        <v>https://www.eia.gov/environment/emissions/co2_vol_mass.php</v>
+      </c>
+      <c r="F27">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="str">
+        <f>Fuels_rawUSD!A28</f>
+        <v>naturalgas_6MMbtu</v>
+      </c>
+      <c r="B28">
+        <f>Fuels_rawUSD!B28*inflator_2017</f>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="C28">
+        <f>Fuels_rawUSD!C28</f>
+        <v>53.07</v>
+      </c>
+      <c r="D28">
+        <f>Fuels_rawUSD!D28</f>
+        <v>0</v>
+      </c>
+      <c r="E28" t="str">
+        <f>Fuels_rawUSD!E28</f>
+        <v>https://www.eia.gov/environment/emissions/co2_vol_mass.php</v>
+      </c>
+      <c r="F28">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="str">
+        <f>Fuels_rawUSD!A29</f>
+        <v>naturalgas_7MMbtu</v>
+      </c>
+      <c r="B29">
+        <f>Fuels_rawUSD!B29*inflator_2017</f>
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="C29">
+        <f>Fuels_rawUSD!C29</f>
+        <v>53.07</v>
+      </c>
+      <c r="D29">
+        <f>Fuels_rawUSD!D29</f>
+        <v>0</v>
+      </c>
+      <c r="E29" t="str">
+        <f>Fuels_rawUSD!E29</f>
+        <v>https://www.eia.gov/environment/emissions/co2_vol_mass.php</v>
+      </c>
+      <c r="F29">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="str">
+        <f>Fuels_rawUSD!A30</f>
+        <v>naturalgas_8MMbtu</v>
+      </c>
+      <c r="B30">
+        <f>Fuels_rawUSD!B30*inflator_2017</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C30">
+        <f>Fuels_rawUSD!C30</f>
+        <v>53.07</v>
+      </c>
+      <c r="D30">
+        <f>Fuels_rawUSD!D30</f>
+        <v>0</v>
+      </c>
+      <c r="E30" t="str">
+        <f>Fuels_rawUSD!E30</f>
+        <v>https://www.eia.gov/environment/emissions/co2_vol_mass.php</v>
+      </c>
+      <c r="F30">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="str">
+        <f>Fuels_rawUSD!A31</f>
+        <v>naturalgas_9MMbtu</v>
+      </c>
+      <c r="B31">
+        <f>Fuels_rawUSD!B31*inflator_2017</f>
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="C31">
+        <f>Fuels_rawUSD!C31</f>
+        <v>53.07</v>
+      </c>
+      <c r="D31">
+        <f>Fuels_rawUSD!D31</f>
+        <v>0</v>
+      </c>
+      <c r="E31" t="str">
+        <f>Fuels_rawUSD!E31</f>
+        <v>https://www.eia.gov/environment/emissions/co2_vol_mass.php</v>
+      </c>
+      <c r="F31">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="str">
+        <f>Fuels_rawUSD!A32</f>
+        <v>naturalgas_10MMbtu</v>
+      </c>
+      <c r="B32">
+        <f>Fuels_rawUSD!B32*inflator_2017</f>
+        <v>0.01</v>
+      </c>
+      <c r="C32">
+        <f>Fuels_rawUSD!C32</f>
+        <v>53.07</v>
+      </c>
+      <c r="D32">
+        <f>Fuels_rawUSD!D32</f>
+        <v>0</v>
+      </c>
+      <c r="E32" t="str">
+        <f>Fuels_rawUSD!E32</f>
+        <v>https://www.eia.gov/environment/emissions/co2_vol_mass.php</v>
+      </c>
+      <c r="F32">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="str">
+        <f>Fuels_rawUSD!A33</f>
+        <v>coal</v>
+      </c>
+      <c r="B33">
+        <f>Fuels_rawUSD!B33*inflator_2017</f>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C33">
+        <f>Fuels_rawUSD!C33</f>
+        <v>100</v>
+      </c>
+      <c r="D33" t="str">
+        <f>Fuels_rawUSD!D33</f>
+        <v>None</v>
+      </c>
+      <c r="E33" t="str">
+        <f>Fuels_rawUSD!E33</f>
+        <v>None</v>
+      </c>
+      <c r="F33">
         <v>2017</v>
       </c>
     </row>
@@ -5681,7 +6022,7 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
@@ -5690,7 +6031,7 @@
     <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -5707,7 +6048,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -5718,7 +6059,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -5729,7 +6070,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>4.2000000000000003E-2</v>
       </c>
@@ -5746,7 +6087,7 @@
         <v>1.1241149062626099</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D5">
         <v>2011</v>
       </c>
@@ -5754,7 +6095,7 @@
         <v>1.08971765678695</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D6">
         <v>2012</v>
       </c>
@@ -5762,7 +6103,7 @@
         <v>1.06762371838985</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D7">
         <v>2013</v>
       </c>
@@ -5770,7 +6111,7 @@
         <v>1.0522113523096499</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D8">
         <v>2014</v>
       </c>
@@ -5778,7 +6119,7 @@
         <v>1.0354149770208101</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D9">
         <v>2015</v>
       </c>
@@ -5786,7 +6127,7 @@
         <v>1.03418742115544</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D10">
         <v>2016</v>
       </c>
@@ -5794,7 +6135,7 @@
         <v>1.02130354531326</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D11">
         <v>2017</v>
       </c>
@@ -5802,7 +6143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D12">
         <v>2018</v>
       </c>
@@ -5823,7 +6164,7 @@
       <selection activeCell="T4" sqref="T4:T13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
@@ -5845,7 +6186,7 @@
     <col min="18" max="18" width="62.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5907,7 +6248,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -5963,7 +6304,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>21</v>
       </c>
@@ -6016,7 +6357,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>90</v>
       </c>
@@ -6085,7 +6426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>91</v>
       </c>
@@ -6154,7 +6495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>92</v>
       </c>
@@ -6223,7 +6564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>93</v>
       </c>
@@ -6291,7 +6632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>94</v>
       </c>
@@ -6360,7 +6701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>95</v>
       </c>
@@ -6429,7 +6770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>96</v>
       </c>
@@ -6498,7 +6839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>97</v>
       </c>
@@ -6567,7 +6908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>99</v>
       </c>
@@ -6636,7 +6977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>98</v>
       </c>
@@ -6719,7 +7060,7 @@
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
@@ -6741,7 +7082,7 @@
     <col min="18" max="18" width="62.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6804,7 +7145,7 @@
         <v>reserves</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -6861,7 +7202,7 @@
         <v>Provides reserves</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>21</v>
       </c>
@@ -6915,7 +7256,7 @@
         <v>[boolean]</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f>Storage_rawUSD!A4</f>
         <v>Li_2030_mid_atb_1hr</v>
@@ -6996,7 +7337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f>Storage_rawUSD!A5</f>
         <v>Li_2030_mid_atb_2hr</v>
@@ -7077,7 +7418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f>Storage_rawUSD!A6</f>
         <v>Li_2030_mid_atb_4hr</v>
@@ -7158,7 +7499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f>Storage_rawUSD!A7</f>
         <v>Li_2030_mid_atb_8hr</v>
@@ -7239,7 +7580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f>Storage_rawUSD!A8</f>
         <v>Li_2030_mid_atb_12hr</v>
@@ -7320,7 +7661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
         <f>Storage_rawUSD!A9</f>
         <v>Li_2018_1hr</v>
@@ -7401,7 +7742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f>Storage_rawUSD!A10</f>
         <v>Li_2018_2hr</v>
@@ -7482,7 +7823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
         <f>Storage_rawUSD!A11</f>
         <v>Li_2018_4hr</v>
@@ -7563,7 +7904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
         <f>Storage_rawUSD!A12</f>
         <v>Li_2018_8hr</v>
@@ -7644,7 +7985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
         <f>Storage_rawUSD!A13</f>
         <v>Li_2018_12hr</v>
@@ -7733,14 +8074,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P59"/>
+  <dimension ref="A1:P60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D31" sqref="D31"/>
+      <selection pane="topRight" activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
@@ -7759,7 +8100,7 @@
     <col min="16" max="16" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7810,7 +8151,7 @@
         <v>reserves</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -7855,7 +8196,7 @@
         <v>Provides reserves</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>42</v>
       </c>
@@ -7897,7 +8238,7 @@
         <v>[boolean]</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f>Generators_rawUSD!A4</f>
         <v>OCGT</v>
@@ -7962,7 +8303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f>Generators_rawUSD!A5</f>
         <v>OCGT_2017</v>
@@ -8027,7 +8368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f>Generators_rawUSD!A6</f>
         <v>OCGT_2030_mid</v>
@@ -8092,7 +8433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f>Generators_rawUSD!A7</f>
         <v>OCGT_2030_low</v>
@@ -8157,7 +8498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f>Generators_rawUSD!A8</f>
         <v>OCGT_2040_mid</v>
@@ -8222,7 +8563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
         <f>Generators_rawUSD!A9</f>
         <v>OCGT_2040_low</v>
@@ -8287,7 +8628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f>Generators_rawUSD!A10</f>
         <v>OCGT_2050_mid</v>
@@ -8352,7 +8693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
         <f>Generators_rawUSD!A11</f>
         <v>OCGT_2050_low</v>
@@ -8417,7 +8758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
         <f>Generators_rawUSD!A12</f>
         <v>CCGT</v>
@@ -8482,7 +8823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
         <f>Generators_rawUSD!A13</f>
         <v>CCGT_2017</v>
@@ -8547,7 +8888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="str">
         <f>Generators_rawUSD!A14</f>
         <v>CCGT_2030_mid</v>
@@ -8612,7 +8953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
         <f>Generators_rawUSD!A15</f>
         <v>CCGT_2030_low</v>
@@ -8677,7 +9018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
         <f>Generators_rawUSD!A16</f>
         <v>CCGT_2040_mid</v>
@@ -8742,7 +9083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="str">
         <f>Generators_rawUSD!A17</f>
         <v>CCGT_2040_low</v>
@@ -8807,7 +9148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
         <f>Generators_rawUSD!A18</f>
         <v>CCGT_2050_mid</v>
@@ -8872,7 +9213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" t="str">
         <f>Generators_rawUSD!A19</f>
         <v>CCGT_2050_low</v>
@@ -8937,7 +9278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="str">
         <f>Generators_rawUSD!A20</f>
         <v>Nuclear</v>
@@ -9002,7 +9343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="str">
         <f>Generators_rawUSD!A21</f>
         <v>Nuclear_2017</v>
@@ -9067,7 +9408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="str">
         <f>Generators_rawUSD!A22</f>
         <v>Nuclear_2030</v>
@@ -9132,7 +9473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
         <f>Generators_rawUSD!A23</f>
         <v>Nuclear_2040</v>
@@ -9197,7 +9538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="str">
         <f>Generators_rawUSD!A24</f>
         <v>Nuclear_2050</v>
@@ -9262,7 +9603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="str">
         <f>Generators_rawUSD!A25</f>
         <v>Nuclear_existing</v>
@@ -9327,7 +9668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" t="str">
         <f>Generators_rawUSD!A26</f>
         <v>Nuclear_vogtle</v>
@@ -9392,7 +9733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" t="str">
         <f>Generators_rawUSD!A27</f>
         <v>Lostload</v>
@@ -9457,7 +9798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" t="str">
         <f>Generators_rawUSD!A28</f>
         <v>PV_track</v>
@@ -9522,7 +9863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" t="str">
         <f>Generators_rawUSD!A29</f>
         <v>PV_fixed</v>
@@ -9587,7 +9928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" t="str">
         <f>Generators_rawUSD!A30</f>
         <v>PV_track_2017</v>
@@ -9652,7 +9993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" t="str">
         <f>Generators_rawUSD!A31</f>
         <v>PV_track_2025_mid</v>
@@ -9717,7 +10058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" t="str">
         <f>Generators_rawUSD!A32</f>
         <v>PV_track_2025_low</v>
@@ -9782,7 +10123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" t="str">
         <f>Generators_rawUSD!A33</f>
         <v>PV_track_2030_mid</v>
@@ -9847,7 +10188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" t="str">
         <f>Generators_rawUSD!A34</f>
         <v>PV_track_2030_low</v>
@@ -9912,7 +10253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" t="str">
         <f>Generators_rawUSD!A35</f>
         <v>PV_track_2040_mid</v>
@@ -9977,7 +10318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" t="str">
         <f>Generators_rawUSD!A36</f>
         <v>PV_track_2040_low</v>
@@ -10042,7 +10383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" t="str">
         <f>Generators_rawUSD!A37</f>
         <v>PV_track_2050_mid</v>
@@ -10107,7 +10448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:16">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" t="str">
         <f>Generators_rawUSD!A38</f>
         <v>PV_track_2050_low</v>
@@ -10172,7 +10513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:16">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" t="str">
         <f>Generators_rawUSD!A39</f>
         <v>Wind</v>
@@ -10237,7 +10578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" t="str">
         <f>Generators_rawUSD!A40</f>
         <v>Wind_2017</v>
@@ -10302,7 +10643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" t="str">
         <f>Generators_rawUSD!A41</f>
         <v>Wind_2025_mid</v>
@@ -10367,7 +10708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:16">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" t="str">
         <f>Generators_rawUSD!A42</f>
         <v>Wind_2025_low</v>
@@ -10432,7 +10773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" t="str">
         <f>Generators_rawUSD!A43</f>
         <v>Wind_2030_mid</v>
@@ -10497,7 +10838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:16">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" t="str">
         <f>Generators_rawUSD!A44</f>
         <v>Wind_2030_low</v>
@@ -10562,7 +10903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:16">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" t="str">
         <f>Generators_rawUSD!A45</f>
         <v>Wind_2040_mid</v>
@@ -10627,7 +10968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:16">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" t="str">
         <f>Generators_rawUSD!A46</f>
         <v>Wind_2040_low</v>
@@ -10692,7 +11033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:16">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" t="str">
         <f>Generators_rawUSD!A47</f>
         <v>Wind_2050_mid</v>
@@ -10757,7 +11098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:16">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" t="str">
         <f>Generators_rawUSD!A48</f>
         <v>Wind_2050_low</v>
@@ -10822,7 +11163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:16">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" t="str">
         <f>Generators_rawUSD!A49</f>
         <v>Wind_off</v>
@@ -10887,7 +11228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:16">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" t="str">
         <f>Generators_rawUSD!A50</f>
         <v>Wind_off_2017</v>
@@ -10952,7 +11293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:16">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" t="str">
         <f>Generators_rawUSD!A51</f>
         <v>Wind_off_2030_mid</v>
@@ -11017,7 +11358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:16">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" t="str">
         <f>Generators_rawUSD!A52</f>
         <v>Wind_off_2030_low</v>
@@ -11082,7 +11423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:16">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" t="str">
         <f>Generators_rawUSD!A53</f>
         <v>Wind_off_2040_mid</v>
@@ -11147,7 +11488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:16">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" t="str">
         <f>Generators_rawUSD!A54</f>
         <v>Wind_off_2040_low</v>
@@ -11212,7 +11553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:16">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" t="str">
         <f>Generators_rawUSD!A55</f>
         <v>Wind_off_2050_mid</v>
@@ -11277,7 +11618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:16">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56" t="str">
         <f>Generators_rawUSD!A56</f>
         <v>Wind_off_2050_low</v>
@@ -11342,7 +11683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:16">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57" t="str">
         <f>Generators_rawUSD!A57</f>
         <v>Hydro_ROR</v>
@@ -11407,7 +11748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:16">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58" t="str">
         <f>Generators_rawUSD!A58</f>
         <v>Nuclear_4</v>
@@ -11472,7 +11813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:16">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59" t="str">
         <f>Generators_rawUSD!A59</f>
         <v>Nuclear_5</v>
@@ -11494,7 +11835,7 @@
         <v>6.7439028038694573E-2</v>
       </c>
       <c r="F59">
-        <f t="shared" ref="F59" si="6">B59*E59</f>
+        <f t="shared" ref="F59:F60" si="6">B59*E59</f>
         <v>337.19514019347287</v>
       </c>
       <c r="G59">
@@ -11534,6 +11875,69 @@
       </c>
       <c r="P59">
         <f>Generators_rawUSD!P59</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A60" t="str">
+        <f>Generators_rawUSD!A60</f>
+        <v>Coal</v>
+      </c>
+      <c r="B60">
+        <v>3000</v>
+      </c>
+      <c r="C60">
+        <f>Generators_rawUSD!C60</f>
+        <v>25</v>
+      </c>
+      <c r="D60">
+        <f>Generators_rawUSD!D60</f>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E60">
+        <f t="shared" ref="E60" si="7">((D60*(1+D60)^C60)/((1+D60)^C60-1))</f>
+        <v>6.7439028038694573E-2</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="6"/>
+        <v>202.31708411608372</v>
+      </c>
+      <c r="G60">
+        <f>Generators_rawUSD!G60*inflator_2017</f>
+        <v>11</v>
+      </c>
+      <c r="H60">
+        <f>Generators_rawUSD!H60*inflator_2017</f>
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="I60">
+        <v>10</v>
+      </c>
+      <c r="J60">
+        <f>Generators_rawUSD!J60</f>
+        <v>0.25</v>
+      </c>
+      <c r="K60">
+        <f>Generators_rawUSD!K60</f>
+        <v>0.25</v>
+      </c>
+      <c r="L60">
+        <f>Generators_rawUSD!L60</f>
+        <v>0</v>
+      </c>
+      <c r="M60" t="str">
+        <f>Generators_rawUSD!M60</f>
+        <v>coal</v>
+      </c>
+      <c r="N60" t="str">
+        <f>Generators_rawUSD!N60</f>
+        <v>None</v>
+      </c>
+      <c r="O60">
+        <v>2017</v>
+      </c>
+      <c r="P60">
+        <f>Generators_rawUSD!P60</f>
         <v>1</v>
       </c>
     </row>
@@ -11551,7 +11955,7 @@
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.83203125" customWidth="1"/>
@@ -11568,7 +11972,7 @@
     <col min="13" max="13" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>206</v>
       </c>
@@ -11612,7 +12016,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>206</v>
       </c>
@@ -11650,7 +12054,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>205</v>
       </c>
@@ -11688,7 +12092,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>230</v>
       </c>
@@ -11732,7 +12136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>345</v>
       </c>
@@ -11776,7 +12180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>500</v>
       </c>
@@ -11820,7 +12224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>765</v>
       </c>
@@ -11864,7 +12268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>212</v>
       </c>
@@ -11922,7 +12326,7 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
@@ -11938,7 +12342,7 @@
     <col min="13" max="13" width="6.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>206</v>
       </c>
@@ -11985,7 +12389,7 @@
         <v>reserves</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>206</v>
       </c>
@@ -12026,7 +12430,7 @@
         <v>Provides reserves</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>205</v>
       </c>
@@ -12067,7 +12471,7 @@
         <v>[boolean]</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
         <f>Transmission_raw!A4</f>
         <v>230</v>
@@ -12120,7 +12524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5">
         <f>Transmission_raw!A5</f>
         <v>345</v>
@@ -12173,7 +12577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
         <f>Transmission_raw!A6</f>
         <v>500</v>
@@ -12226,7 +12630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
         <f>Transmission_raw!A7</f>
         <v>765</v>
@@ -12279,7 +12683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f>Transmission_raw!A8</f>
         <v>DC</v>
@@ -12345,7 +12749,7 @@
       <selection activeCell="P1" sqref="P1:P5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
@@ -12363,7 +12767,7 @@
     <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -12413,7 +12817,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -12457,7 +12861,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>42</v>
       </c>
@@ -12498,7 +12902,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>202</v>
       </c>
@@ -12550,7 +12954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>201</v>
       </c>
@@ -12615,7 +13019,7 @@
       <selection activeCell="P1" sqref="P1:P5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
@@ -12633,7 +13037,7 @@
     <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -12684,7 +13088,7 @@
         <v>reserves</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -12729,7 +13133,7 @@
         <v>Provides reserves</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>42</v>
       </c>
@@ -12771,7 +13175,7 @@
         <v>[boolean]</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f>Hydro_rawUSD!A4</f>
         <v>Hydro_Res</v>
@@ -12836,7 +13240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f>Hydro_rawUSD!A5</f>
         <v>Hydro_ROR</v>
@@ -12914,9 +13318,9 @@
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>188</v>
       </c>
@@ -12936,7 +13340,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>149</v>
       </c>
@@ -12962,7 +13366,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>153</v>
       </c>
@@ -12975,20 +13379,20 @@
       <c r="D3" s="2">
         <v>1</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3">
         <v>380</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3">
         <v>380</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3">
         <v>380</v>
       </c>
       <c r="H3" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>154</v>
       </c>
@@ -13001,20 +13405,20 @@
       <c r="D4" s="2">
         <v>0.97</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4">
         <v>339</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4">
         <v>355</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4">
         <v>369</v>
       </c>
       <c r="H4" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -13027,20 +13431,20 @@
       <c r="D5" s="2">
         <v>0.94</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5">
         <v>297</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5">
         <v>330</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5">
         <v>359</v>
       </c>
       <c r="H5" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>156</v>
       </c>
@@ -13053,20 +13457,20 @@
       <c r="D6" s="2">
         <v>0.93</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6">
         <v>275</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6">
         <v>313</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6">
         <v>353</v>
       </c>
       <c r="H6" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>157</v>
       </c>
@@ -13079,20 +13483,20 @@
       <c r="D7" s="2">
         <v>0.91</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7">
         <v>252</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7">
         <v>297</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7">
         <v>347</v>
       </c>
       <c r="H7" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>158</v>
       </c>
@@ -13105,20 +13509,20 @@
       <c r="D8" s="2">
         <v>0.9</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8">
         <v>229</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8">
         <v>280</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8">
         <v>341</v>
       </c>
       <c r="H8" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>159</v>
       </c>
@@ -13131,20 +13535,20 @@
       <c r="D9" s="2">
         <v>0.88</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9">
         <v>207</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9">
         <v>264</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9">
         <v>336</v>
       </c>
       <c r="H9" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>160</v>
       </c>
@@ -13157,20 +13561,20 @@
       <c r="D10" s="2">
         <v>0.87</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10">
         <v>184</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10">
         <v>248</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10">
         <v>330</v>
       </c>
       <c r="H10" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>161</v>
       </c>
@@ -13183,20 +13587,20 @@
       <c r="D11" s="2">
         <v>0.85</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11">
         <v>172</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11">
         <v>240</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11">
         <v>324</v>
       </c>
       <c r="H11" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>162</v>
       </c>
@@ -13209,20 +13613,20 @@
       <c r="D12" s="2">
         <v>0.84</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12">
         <v>160</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12">
         <v>232</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12">
         <v>318</v>
       </c>
       <c r="H12" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>163</v>
       </c>
@@ -13235,20 +13639,20 @@
       <c r="D13" s="2">
         <v>0.82</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13">
         <v>148</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13">
         <v>224</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13">
         <v>312</v>
       </c>
       <c r="H13" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>164</v>
       </c>
@@ -13261,20 +13665,20 @@
       <c r="D14" s="2">
         <v>0.81</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14">
         <v>136</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14">
         <v>215</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14">
         <v>307</v>
       </c>
       <c r="H14" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>165</v>
       </c>
@@ -13287,20 +13691,20 @@
       <c r="D15" s="2">
         <v>0.79</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15">
         <v>124</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15">
         <v>207</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15">
         <v>301</v>
       </c>
       <c r="H15" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>166</v>
       </c>
@@ -13313,20 +13717,20 @@
       <c r="D16" s="2">
         <v>0.79</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16">
         <v>122</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16">
         <v>205</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16">
         <v>299</v>
       </c>
       <c r="H16" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>167</v>
       </c>
@@ -13339,20 +13743,20 @@
       <c r="D17" s="2">
         <v>0.78</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17">
         <v>120</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17">
         <v>202</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17">
         <v>297</v>
       </c>
       <c r="H17" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>168</v>
       </c>
@@ -13365,20 +13769,20 @@
       <c r="D18" s="2">
         <v>0.78</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18">
         <v>117</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18">
         <v>200</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G18">
         <v>295</v>
       </c>
       <c r="H18" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>169</v>
       </c>
@@ -13391,20 +13795,20 @@
       <c r="D19" s="2">
         <v>0.77</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19">
         <v>115</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19">
         <v>197</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19">
         <v>293</v>
       </c>
       <c r="H19" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>170</v>
       </c>
@@ -13417,20 +13821,20 @@
       <c r="D20" s="2">
         <v>0.77</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20">
         <v>112</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20">
         <v>194</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20">
         <v>291</v>
       </c>
       <c r="H20" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>171</v>
       </c>
@@ -13443,20 +13847,20 @@
       <c r="D21" s="2">
         <v>0.76</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21">
         <v>110</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21">
         <v>192</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21">
         <v>290</v>
       </c>
       <c r="H21" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>172</v>
       </c>
@@ -13469,20 +13873,20 @@
       <c r="D22" s="2">
         <v>0.76</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22">
         <v>107</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22">
         <v>189</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G22">
         <v>288</v>
       </c>
       <c r="H22" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>173</v>
       </c>
@@ -13495,20 +13899,20 @@
       <c r="D23" s="2">
         <v>0.75</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23">
         <v>105</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23">
         <v>187</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G23">
         <v>286</v>
       </c>
       <c r="H23" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>174</v>
       </c>
@@ -13521,20 +13925,20 @@
       <c r="D24" s="2">
         <v>0.75</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24">
         <v>102</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24">
         <v>184</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G24">
         <v>284</v>
       </c>
       <c r="H24" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>175</v>
       </c>
@@ -13547,20 +13951,20 @@
       <c r="D25" s="2">
         <v>0.74</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25">
         <v>100</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25">
         <v>182</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G25">
         <v>282</v>
       </c>
       <c r="H25" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>176</v>
       </c>
@@ -13573,20 +13977,20 @@
       <c r="D26" s="2">
         <v>0.74</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26">
         <v>98</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26">
         <v>179</v>
       </c>
-      <c r="G26" s="3">
+      <c r="G26">
         <v>280</v>
       </c>
       <c r="H26" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>177</v>
       </c>
@@ -13599,20 +14003,20 @@
       <c r="D27" s="2">
         <v>0.73</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27">
         <v>95</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27">
         <v>176</v>
       </c>
-      <c r="G27" s="3">
+      <c r="G27">
         <v>278</v>
       </c>
       <c r="H27" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>178</v>
       </c>
@@ -13625,20 +14029,20 @@
       <c r="D28" s="2">
         <v>0.73</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28">
         <v>93</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28">
         <v>174</v>
       </c>
-      <c r="G28" s="3">
+      <c r="G28">
         <v>276</v>
       </c>
       <c r="H28" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>179</v>
       </c>
@@ -13651,20 +14055,20 @@
       <c r="D29" s="2">
         <v>0.72</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29">
         <v>90</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F29">
         <v>171</v>
       </c>
-      <c r="G29" s="3">
+      <c r="G29">
         <v>274</v>
       </c>
       <c r="H29" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>180</v>
       </c>
@@ -13677,20 +14081,20 @@
       <c r="D30" s="2">
         <v>0.72</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30">
         <v>88</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F30">
         <v>169</v>
       </c>
-      <c r="G30" s="3">
+      <c r="G30">
         <v>273</v>
       </c>
       <c r="H30" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>181</v>
       </c>
@@ -13703,20 +14107,20 @@
       <c r="D31" s="2">
         <v>0.71</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31">
         <v>85</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F31">
         <v>166</v>
       </c>
-      <c r="G31" s="3">
+      <c r="G31">
         <v>271</v>
       </c>
       <c r="H31" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>182</v>
       </c>
@@ -13729,20 +14133,20 @@
       <c r="D32" s="2">
         <v>0.71</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32">
         <v>83</v>
       </c>
-      <c r="F32" s="3">
+      <c r="F32">
         <v>163</v>
       </c>
-      <c r="G32" s="3">
+      <c r="G32">
         <v>269</v>
       </c>
       <c r="H32" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>183</v>
       </c>
@@ -13755,20 +14159,20 @@
       <c r="D33" s="2">
         <v>0.7</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E33">
         <v>81</v>
       </c>
-      <c r="F33" s="3">
+      <c r="F33">
         <v>161</v>
       </c>
-      <c r="G33" s="3">
+      <c r="G33">
         <v>267</v>
       </c>
       <c r="H33" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>184</v>
       </c>
@@ -13781,20 +14185,20 @@
       <c r="D34" s="2">
         <v>0.7</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34">
         <v>78</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F34">
         <v>158</v>
       </c>
-      <c r="G34" s="3">
+      <c r="G34">
         <v>265</v>
       </c>
       <c r="H34" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>190</v>
       </c>
@@ -13807,13 +14211,13 @@
       <c r="D35" s="2">
         <v>0.69</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E35">
         <v>76</v>
       </c>
-      <c r="F35" s="3">
+      <c r="F35">
         <v>156</v>
       </c>
-      <c r="G35" s="3">
+      <c r="G35">
         <v>263</v>
       </c>
       <c r="H35" t="s">
@@ -13833,7 +14237,7 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
@@ -13857,7 +14261,7 @@
     <col min="20" max="20" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -13922,7 +14326,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -13981,7 +14385,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>28</v>
       </c>
@@ -14037,7 +14441,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>82</v>
       </c>
@@ -14107,7 +14511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -14181,7 +14585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>69</v>
       </c>
@@ -14255,7 +14659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>70</v>
       </c>
@@ -14329,7 +14733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>185</v>
       </c>
@@ -14403,7 +14807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>71</v>
       </c>
@@ -14477,7 +14881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -14551,7 +14955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>73</v>
       </c>
@@ -14625,7 +15029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>74</v>
       </c>
@@ -14699,7 +15103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>186</v>
       </c>
@@ -14773,7 +15177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>75</v>
       </c>
@@ -14847,7 +15251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>192</v>
       </c>
@@ -14917,7 +15321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>194</v>
       </c>
@@ -14987,7 +15391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>265</v>
       </c>
@@ -15059,7 +15463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>267</v>
       </c>
@@ -15130,7 +15534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>269</v>
       </c>
@@ -15201,7 +15605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>282</v>
       </c>
@@ -15284,7 +15688,7 @@
       <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
@@ -15308,7 +15712,7 @@
     <col min="20" max="20" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
         <f>Storage_variable_rawUSD!A1</f>
         <v>Technology</v>
@@ -15392,7 +15796,7 @@
         <v>reserves</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>Storage_variable_rawUSD!A2</f>
         <v>Technology</v>
@@ -15469,7 +15873,7 @@
         <v>Provides reserves</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>Storage_variable_rawUSD!A3</f>
         <v>0</v>
@@ -15546,7 +15950,7 @@
         <v>[boolean]</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f>Storage_variable_rawUSD!A4</f>
         <v>Li_2018</v>
@@ -15631,7 +16035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f>Storage_variable_rawUSD!A5</f>
         <v>Li_2020_mid</v>
@@ -15716,7 +16120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f>Storage_variable_rawUSD!A6</f>
         <v>Li_2025_mid</v>
@@ -15801,7 +16205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f>Storage_variable_rawUSD!A7</f>
         <v>Li_2030_mid</v>
@@ -15886,7 +16290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f>Storage_variable_rawUSD!A8</f>
         <v>Li_2040_mid</v>
@@ -15971,7 +16375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
         <f>Storage_variable_rawUSD!A9</f>
         <v>Li_2050_mid</v>
@@ -16056,7 +16460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f>Storage_variable_rawUSD!A10</f>
         <v>Li_2020_low</v>
@@ -16141,7 +16545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
         <f>Storage_variable_rawUSD!A11</f>
         <v>Li_2025_low</v>
@@ -16226,7 +16630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
         <f>Storage_variable_rawUSD!A12</f>
         <v>Li_2030_low</v>
@@ -16311,7 +16715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
         <f>Storage_variable_rawUSD!A13</f>
         <v>Li_2040_low</v>
@@ -16396,7 +16800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" t="str">
         <f>Storage_variable_rawUSD!A14</f>
         <v>Li_2050_low</v>
@@ -16481,7 +16885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
         <f>Storage_variable_rawUSD!A15</f>
         <v>PHS</v>
@@ -16566,7 +16970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
         <f>Storage_variable_rawUSD!A16</f>
         <v>PHS_low</v>
@@ -16651,7 +17055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" t="str">
         <f>Storage_variable_rawUSD!A17</f>
         <v>Li_2018_5x</v>
@@ -16736,7 +17140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
         <f>Storage_variable_rawUSD!A18</f>
         <v>PHS_20</v>
@@ -16821,7 +17225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" t="str">
         <f>Storage_variable_rawUSD!A19</f>
         <v>PHS_10</v>
@@ -16906,7 +17310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" t="str">
         <f>Storage_variable_rawUSD!A20</f>
         <v>PHS_0</v>

</xml_diff>